<commit_message>
new computation of zipf-mandelbrot estimate
</commit_message>
<xml_diff>
--- a/results/real_corpora/real_corpora_correlation.xlsx
+++ b/results/real_corpora/real_corpora_correlation.xlsx
@@ -35,7 +35,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="92">
+  <fills count="91">
     <fill>
       <patternFill/>
     </fill>
@@ -59,142 +59,327 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="007A9DF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00799CF8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="006384EB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EDD2C3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0096B7FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003B4CC0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F2CBB7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004055C8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDDCDC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F29072"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F59D7E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F5C1A9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0089ACFD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EED0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E4D9D2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7A98B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C5D6F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004961D2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6D7CF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D8DCE2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EC8165"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B70D28"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E0DBD8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BD1F2D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C9D7F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D65244"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D1493F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005673E0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E3D9D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BCD2F7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B8122A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CB3E38"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005D7CE6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004E68D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="006485EC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008CAFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="008BADFD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0080A3FA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0092B4FE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="009ABBFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006384EB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EDD2C3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0096B7FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003B4CC0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F2CBB7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004055C8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DDDCDC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F29072"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F59D7E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F5C2AA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EED0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E4D9D2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7A98B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C5D6F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004961D2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E6D7CF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D8DCE2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EC8165"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B70D28"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006F92F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BD1F2D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C9D7F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D65244"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D1493F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005673E0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007699F6"/>
+        <fgColor rgb="0082A6FB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="003D50C3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7AA8C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2DAD5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00AEC9FC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C12B30"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C43032"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005875E1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1CDBA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EBD3C6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007B9FF9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BFD3F6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005E7DE7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009EBEFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DFDBD9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005470DE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D1DAE9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F08A6C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BA162B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CEDAEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009FBFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D44E41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CA3B37"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005A78E4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F59F80"/>
       </patternFill>
     </fill>
     <fill>
@@ -204,42 +389,62 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BA162B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CB3E38"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005D7CE6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B9D0F9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006E90F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004358CB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003F53C6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A9C6FD"/>
+        <fgColor rgb="006180E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CAD8EF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7B99E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005F7FE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004B64D5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C83836"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B1CBFC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F7AC8E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CD423B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C32E31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B5CDFA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CF453C"/>
       </patternFill>
     </fill>
     <fill>
@@ -249,216 +454,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="003D50C3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F5C1A9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="003E51C5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00BCD2F7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7AA8C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00AEC9FC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C12B30"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C43032"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005875E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F1CDBA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00EBD3C6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007A9DF8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0094B6FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005E7DE7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009EBEFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DFDBD9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005470DE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D1DAE9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F08A6C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00779AF7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CEDAEB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="009FBFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D44E41"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CA3B37"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="007EA1FA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0092B4FE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005A78E4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F59F80"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="006180E9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F6A385"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004E68D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7B99E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="005F7FE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004B64D5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C83836"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B1CBFC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7AC8E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CD423B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="008FB1FE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00C32E31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00B5CDFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CF453C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00F7BCA1"/>
       </patternFill>
     </fill>
@@ -474,12 +469,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00688AEF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F7B396"/>
+        <fgColor rgb="006A8BEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C1D4F4"/>
       </patternFill>
     </fill>
     <fill>
@@ -511,101 +506,100 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="84" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="70" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="78" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="85" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="38" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="47" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="53" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="61" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="39" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="65" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="71" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="80" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="79" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="86" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="40" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="54" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="66" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="77" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="62" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="55" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="67" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="52" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="87" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="72" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="88" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="80" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="89" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="64" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="81" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="89" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="56" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="49" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="73" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="82" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="90" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="48" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="63" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="74" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="83" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="42" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="57" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="75" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="84" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="91" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="43" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="37" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="60" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="46" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="68" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="76" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="44" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="58" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="45" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="50" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="59" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="51" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="69" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="83" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1057,10 +1051,10 @@
         <v>0.1073281433167386</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>-0.0443912427396965</v>
+        <v>-0.04315214995590905</v>
       </c>
       <c r="F2" s="6" t="n">
-        <v>0.07708894084123194</v>
+        <v>-0.04780758853382465</v>
       </c>
       <c r="G2" s="7" t="n">
         <v>-0.1293362860187998</v>
@@ -1100,10 +1094,10 @@
         <v>0.6689757318979073</v>
       </c>
       <c r="E3" s="16" t="n">
-        <v>0.5322286114651112</v>
+        <v>0.5332082151251626</v>
       </c>
       <c r="F3" s="17" t="n">
-        <v>-0.2429684394058505</v>
+        <v>0.03277220354819806</v>
       </c>
       <c r="G3" s="18" t="n">
         <v>0.4589923738906266</v>
@@ -1143,10 +1137,10 @@
         <v>1</v>
       </c>
       <c r="E4" s="26" t="n">
-        <v>0.984434582038183</v>
+        <v>0.9845111993230353</v>
       </c>
       <c r="F4" s="27" t="n">
-        <v>-0.4398787869896921</v>
+        <v>0.1574705134718265</v>
       </c>
       <c r="G4" s="28" t="n">
         <v>0.9544236257252072</v>
@@ -1177,40 +1171,40 @@
         </is>
       </c>
       <c r="B5" s="34" t="n">
-        <v>-0.0443912427396965</v>
+        <v>-0.04315214995590905</v>
       </c>
       <c r="C5" s="35" t="n">
-        <v>0.5322286114651112</v>
+        <v>0.5332082151251626</v>
       </c>
       <c r="D5" s="26" t="n">
-        <v>0.9844345820381829</v>
+        <v>0.9845111993230353</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="F5" s="36" t="n">
-        <v>-0.4581702611901197</v>
+        <v>0.1523883832489007</v>
       </c>
       <c r="G5" s="26" t="n">
-        <v>0.9843902809486744</v>
+        <v>0.9841806201409633</v>
       </c>
       <c r="H5" s="37" t="n">
-        <v>-0.09738515981246612</v>
+        <v>-0.09277823612918745</v>
       </c>
       <c r="I5" s="38" t="n">
-        <v>0.9709895199286411</v>
+        <v>0.9722084319172892</v>
       </c>
       <c r="J5" s="39" t="n">
-        <v>0.8859410063917093</v>
+        <v>0.8868829465657287</v>
       </c>
       <c r="K5" s="40" t="n">
-        <v>-0.7876354706066507</v>
-      </c>
-      <c r="L5" s="41" t="n">
-        <v>0.8856601335833322</v>
-      </c>
-      <c r="M5" s="42" t="n">
-        <v>-0.5916932066423126</v>
+        <v>-0.7847965906545162</v>
+      </c>
+      <c r="L5" s="39" t="n">
+        <v>0.8825432784039708</v>
+      </c>
+      <c r="M5" s="41" t="n">
+        <v>-0.5883997960299941</v>
       </c>
     </row>
     <row r="6">
@@ -1219,41 +1213,41 @@
           <t>sd_subsample_entropy_rdm</t>
         </is>
       </c>
-      <c r="B6" s="43" t="n">
-        <v>0.07708894084123195</v>
-      </c>
-      <c r="C6" s="44" t="n">
-        <v>-0.2429684394058505</v>
-      </c>
-      <c r="D6" s="45" t="n">
-        <v>-0.4398787869896921</v>
-      </c>
-      <c r="E6" s="46" t="n">
-        <v>-0.4581702611901197</v>
+      <c r="B6" s="42" t="n">
+        <v>-0.04780758853382465</v>
+      </c>
+      <c r="C6" s="43" t="n">
+        <v>0.03277220354819806</v>
+      </c>
+      <c r="D6" s="44" t="n">
+        <v>0.1574705134718265</v>
+      </c>
+      <c r="E6" s="45" t="n">
+        <v>0.1523883832489007</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="34" t="n">
-        <v>-0.4841218854673612</v>
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="G6" s="46" t="n">
+        <v>0.1198573200934725</v>
       </c>
       <c r="H6" s="47" t="n">
-        <v>0.006216768290464615</v>
+        <v>0.1746552770105018</v>
       </c>
       <c r="I6" s="48" t="n">
-        <v>-0.4036762184185549</v>
+        <v>0.1997119242968409</v>
       </c>
       <c r="J6" s="49" t="n">
-        <v>-0.4701172867021736</v>
+        <v>0.1259522777236924</v>
       </c>
       <c r="K6" s="50" t="n">
-        <v>0.458851491988472</v>
+        <v>-0.1201286305658291</v>
       </c>
       <c r="L6" s="51" t="n">
-        <v>-0.4647823871153144</v>
+        <v>0.148429146912695</v>
       </c>
       <c r="M6" s="52" t="n">
-        <v>0.4064731886785423</v>
+        <v>-0.109939089950391</v>
       </c>
     </row>
     <row r="7">
@@ -1272,10 +1266,10 @@
         <v>0.9544236257252072</v>
       </c>
       <c r="E7" s="26" t="n">
-        <v>0.9843902809486743</v>
+        <v>0.9841806201409633</v>
       </c>
       <c r="F7" s="55" t="n">
-        <v>-0.4841218854673612</v>
+        <v>0.1198573200934726</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>0.9999999999999998</v>
@@ -1289,13 +1283,13 @@
       <c r="J7" s="57" t="n">
         <v>0.9317584764439572</v>
       </c>
-      <c r="K7" s="58" t="n">
+      <c r="K7" s="6" t="n">
         <v>-0.8439035884853963</v>
       </c>
-      <c r="L7" s="59" t="n">
+      <c r="L7" s="58" t="n">
         <v>0.920121488762621</v>
       </c>
-      <c r="M7" s="60" t="n">
+      <c r="M7" s="59" t="n">
         <v>-0.6683295614890353</v>
       </c>
     </row>
@@ -1305,37 +1299,37 @@
           <t>sd_subsample_entropy_mav</t>
         </is>
       </c>
-      <c r="B8" s="61" t="n">
+      <c r="B8" s="51" t="n">
         <v>0.4411309126039535</v>
       </c>
-      <c r="C8" s="62" t="n">
+      <c r="C8" s="49" t="n">
         <v>0.3989610804208928</v>
       </c>
-      <c r="D8" s="63" t="n">
+      <c r="D8" s="60" t="n">
         <v>0.01062927370481121</v>
       </c>
-      <c r="E8" s="22" t="n">
-        <v>-0.09738515981246612</v>
-      </c>
-      <c r="F8" s="64" t="n">
-        <v>0.006216768290464614</v>
-      </c>
-      <c r="G8" s="65" t="n">
+      <c r="E8" s="7" t="n">
+        <v>-0.09277823612918745</v>
+      </c>
+      <c r="F8" s="61" t="n">
+        <v>0.1746552770105018</v>
+      </c>
+      <c r="G8" s="62" t="n">
         <v>-0.2077012350935809</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="66" t="n">
+      <c r="I8" s="63" t="n">
         <v>0.04165829076194076</v>
       </c>
-      <c r="J8" s="67" t="n">
+      <c r="J8" s="61" t="n">
         <v>-0.3669370156983324</v>
       </c>
-      <c r="K8" s="68" t="n">
+      <c r="K8" s="64" t="n">
         <v>0.3322314791635443</v>
       </c>
-      <c r="L8" s="69" t="n">
+      <c r="L8" s="65" t="n">
         <v>-0.25208614270923</v>
       </c>
       <c r="M8" s="21" t="n">
@@ -1351,22 +1345,22 @@
       <c r="B9" s="29" t="n">
         <v>0.05747309664118889</v>
       </c>
-      <c r="C9" s="70" t="n">
+      <c r="C9" s="66" t="n">
         <v>0.6284914435775282</v>
       </c>
       <c r="D9" s="26" t="n">
         <v>0.9833677994910359</v>
       </c>
-      <c r="E9" s="38" t="n">
-        <v>0.9709895199286412</v>
-      </c>
-      <c r="F9" s="71" t="n">
-        <v>-0.4036762184185549</v>
+      <c r="E9" s="67" t="n">
+        <v>0.9722084319172892</v>
+      </c>
+      <c r="F9" s="68" t="n">
+        <v>0.1997119242968409</v>
       </c>
       <c r="G9" s="57" t="n">
         <v>0.9325437066496383</v>
       </c>
-      <c r="H9" s="72" t="n">
+      <c r="H9" s="69" t="n">
         <v>0.04165829076194077</v>
       </c>
       <c r="I9" s="2" t="n">
@@ -1375,13 +1369,13 @@
       <c r="J9" s="30" t="n">
         <v>0.8265578038474086</v>
       </c>
-      <c r="K9" s="73" t="n">
+      <c r="K9" s="70" t="n">
         <v>-0.7352175573927546</v>
       </c>
-      <c r="L9" s="74" t="n">
+      <c r="L9" s="71" t="n">
         <v>0.8514545395674457</v>
       </c>
-      <c r="M9" s="75" t="n">
+      <c r="M9" s="72" t="n">
         <v>-0.5381278575780538</v>
       </c>
     </row>
@@ -1391,40 +1385,40 @@
           <t>MTLD</t>
         </is>
       </c>
-      <c r="B10" s="55" t="n">
+      <c r="B10" s="73" t="n">
         <v>-0.2973139288289575</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0.2586313489406851</v>
       </c>
-      <c r="D10" s="76" t="n">
+      <c r="D10" s="74" t="n">
         <v>0.8267900378410771</v>
       </c>
-      <c r="E10" s="77" t="n">
-        <v>0.8859410063917094</v>
-      </c>
-      <c r="F10" s="78" t="n">
-        <v>-0.4701172867021736</v>
+      <c r="E10" s="75" t="n">
+        <v>0.8868829465657287</v>
+      </c>
+      <c r="F10" s="76" t="n">
+        <v>0.1259522777236924</v>
       </c>
       <c r="G10" s="57" t="n">
         <v>0.9317584764439572</v>
       </c>
-      <c r="H10" s="55" t="n">
+      <c r="H10" s="73" t="n">
         <v>-0.3669370156983324</v>
       </c>
-      <c r="I10" s="76" t="n">
+      <c r="I10" s="74" t="n">
         <v>0.8265578038474086</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="K10" s="79" t="n">
+      <c r="K10" s="77" t="n">
         <v>-0.8554867371004373</v>
       </c>
       <c r="L10" s="39" t="n">
         <v>0.8791654961740537</v>
       </c>
-      <c r="M10" s="80" t="n">
+      <c r="M10" s="78" t="n">
         <v>-0.6608429383247335</v>
       </c>
     </row>
@@ -1437,34 +1431,34 @@
       <c r="B11" s="21" t="n">
         <v>0.4825596093146207</v>
       </c>
-      <c r="C11" s="81" t="n">
+      <c r="C11" s="79" t="n">
         <v>-0.2126101228472446</v>
       </c>
-      <c r="D11" s="55" t="n">
+      <c r="D11" s="73" t="n">
         <v>-0.7287527020391559</v>
       </c>
-      <c r="E11" s="55" t="n">
-        <v>-0.7876354706066507</v>
-      </c>
-      <c r="F11" s="82" t="n">
-        <v>0.458851491988472</v>
-      </c>
-      <c r="G11" s="55" t="n">
+      <c r="E11" s="73" t="n">
+        <v>-0.7847965906545162</v>
+      </c>
+      <c r="F11" s="73" t="n">
+        <v>-0.1201286305658291</v>
+      </c>
+      <c r="G11" s="73" t="n">
         <v>-0.8439035884853961</v>
       </c>
-      <c r="H11" s="83" t="n">
+      <c r="H11" s="80" t="n">
         <v>0.3322314791635443</v>
       </c>
-      <c r="I11" s="55" t="n">
+      <c r="I11" s="73" t="n">
         <v>-0.7352175573927547</v>
       </c>
-      <c r="J11" s="55" t="n">
+      <c r="J11" s="73" t="n">
         <v>-0.8554867371004373</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="L11" s="55" t="n">
+      <c r="L11" s="73" t="n">
         <v>-0.9696025932609152</v>
       </c>
       <c r="M11" s="39" t="n">
@@ -1477,40 +1471,40 @@
           <t>zipf_slope</t>
         </is>
       </c>
-      <c r="B12" s="44" t="n">
+      <c r="B12" s="81" t="n">
         <v>-0.2697240840469218</v>
       </c>
-      <c r="C12" s="84" t="n">
+      <c r="C12" s="48" t="n">
         <v>0.413152515724687</v>
       </c>
-      <c r="D12" s="85" t="n">
+      <c r="D12" s="82" t="n">
         <v>0.8571542784054715</v>
       </c>
-      <c r="E12" s="77" t="n">
-        <v>0.8856601335833321</v>
-      </c>
-      <c r="F12" s="86" t="n">
-        <v>-0.4647823871153144</v>
-      </c>
-      <c r="G12" s="87" t="n">
+      <c r="E12" s="75" t="n">
+        <v>0.8825432784039708</v>
+      </c>
+      <c r="F12" s="43" t="n">
+        <v>0.148429146912695</v>
+      </c>
+      <c r="G12" s="83" t="n">
         <v>0.920121488762621</v>
       </c>
-      <c r="H12" s="88" t="n">
+      <c r="H12" s="84" t="n">
         <v>-0.25208614270923</v>
       </c>
-      <c r="I12" s="85" t="n">
+      <c r="I12" s="82" t="n">
         <v>0.8514545395674457</v>
       </c>
-      <c r="J12" s="77" t="n">
+      <c r="J12" s="75" t="n">
         <v>0.8791654961740537</v>
       </c>
-      <c r="K12" s="55" t="n">
+      <c r="K12" s="73" t="n">
         <v>-0.9696025932609151</v>
       </c>
       <c r="L12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="M12" s="55" t="n">
+      <c r="M12" s="73" t="n">
         <v>-0.866729061752828</v>
       </c>
     </row>
@@ -1520,22 +1514,22 @@
           <t>zipf_shift</t>
         </is>
       </c>
-      <c r="B13" s="89" t="n">
+      <c r="B13" s="85" t="n">
         <v>0.3513578804031323</v>
       </c>
-      <c r="C13" s="55" t="n">
+      <c r="C13" s="73" t="n">
         <v>-0.2725841248542779</v>
       </c>
-      <c r="D13" s="40" t="n">
+      <c r="D13" s="86" t="n">
         <v>-0.5691922161340326</v>
       </c>
-      <c r="E13" s="80" t="n">
-        <v>-0.5916932066423125</v>
-      </c>
-      <c r="F13" s="21" t="n">
-        <v>0.4064731886785423</v>
-      </c>
-      <c r="G13" s="90" t="n">
+      <c r="E13" s="78" t="n">
+        <v>-0.588399796029994</v>
+      </c>
+      <c r="F13" s="87" t="n">
+        <v>-0.109939089950391</v>
+      </c>
+      <c r="G13" s="40" t="n">
         <v>-0.6683295614890354</v>
       </c>
       <c r="H13" s="9" t="n">
@@ -1544,13 +1538,13 @@
       <c r="I13" s="56" t="n">
         <v>-0.5381278575780538</v>
       </c>
-      <c r="J13" s="91" t="n">
+      <c r="J13" s="88" t="n">
         <v>-0.6608429383247335</v>
       </c>
-      <c r="K13" s="41" t="n">
+      <c r="K13" s="89" t="n">
         <v>0.8897983151811805</v>
       </c>
-      <c r="L13" s="71" t="n">
+      <c r="L13" s="90" t="n">
         <v>-0.866729061752828</v>
       </c>
       <c r="M13" s="2" t="n">

</xml_diff>